<commit_message>
Rimosso test case 4 laboratorio
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INNOGEASRLX/Innogea srl/CareMed/1.0/accreditamento-checklist_V8.1.2.xlsx
+++ b/GATEWAY/A1#111INNOGEASRLX/Innogea srl/CareMed/1.0/accreditamento-checklist_V8.1.2.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="171">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -352,10 +352,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">26c69d879601c114</t>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.5.4.386ca4745f4026d713155e93f1ffbb24af97a509f18e357ac51281a86f96404d.6d7219c6ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">La codifica SpecimenType per I campioni di laboratorio non è implementata in CareMed. Lo sarà in una prossima release. Questo rende impossibile riprodurre il test case. </t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -424,9 +424,6 @@
       <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Al fine di rendere non valido il token è necessario non valorizzare nel JWT il campo "purpose_of_use".</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Viene effettuata validazione preventiva bloccante sull'applicativo CareMed di tutte le informazioni necessarie a generare un token per l'interazione con i servizi FSE. Se la validazione fallisce non è possibile firmare digitalmente il relativo documento da trasmettere e quindi nessuna trasmissione può essere iniziata.</t>
@@ -1278,9 +1275,9 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="230.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="230.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
   </cols>
   <sheetData>
@@ -2352,7 +2349,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3456,14 +3453,14 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
@@ -3472,9 +3469,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="191.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="0" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="36.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="31.86"/>
@@ -3869,22 +3866,16 @@
       <c r="E13" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="35" t="n">
-        <v>45086</v>
-      </c>
-      <c r="G13" s="30" t="n">
-        <v>20230609155325</v>
-      </c>
-      <c r="H13" s="30" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="30" t="s">
+      <c r="K13" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="31"/>
       <c r="L13" s="31"/>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
@@ -3962,10 +3953,10 @@
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
       <c r="J15" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="28" t="s">
         <v>76</v>
-      </c>
-      <c r="K15" s="28" t="s">
-        <v>77</v>
       </c>
       <c r="L15" s="31"/>
       <c r="M15" s="31"/>
@@ -3976,7 +3967,7 @@
       <c r="R15" s="32"/>
       <c r="S15" s="33"/>
       <c r="T15" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3990,20 +3981,20 @@
         <v>51</v>
       </c>
       <c r="D16" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>79</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>80</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
       <c r="J16" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" s="28" t="s">
         <v>76</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>77</v>
       </c>
       <c r="L16" s="31"/>
       <c r="M16" s="31"/>
@@ -4014,7 +4005,7 @@
       <c r="R16" s="32"/>
       <c r="S16" s="33"/>
       <c r="T16" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4028,17 +4019,17 @@
         <v>51</v>
       </c>
       <c r="D17" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>81</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>82</v>
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
       <c r="J17" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
@@ -4046,13 +4037,13 @@
       <c r="N17" s="31"/>
       <c r="O17" s="31"/>
       <c r="P17" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q17" s="31"/>
       <c r="R17" s="32"/>
       <c r="S17" s="33"/>
       <c r="T17" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4066,20 +4057,20 @@
         <v>51</v>
       </c>
       <c r="D18" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>85</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>86</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
       <c r="J18" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L18" s="31"/>
       <c r="M18" s="31"/>
@@ -4090,7 +4081,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
       <c r="T18" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4104,20 +4095,20 @@
         <v>51</v>
       </c>
       <c r="D19" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>88</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>89</v>
       </c>
       <c r="F19" s="35"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37"/>
       <c r="J19" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L19" s="31"/>
       <c r="M19" s="31"/>
@@ -4128,7 +4119,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
       <c r="T19" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4142,20 +4133,20 @@
         <v>51</v>
       </c>
       <c r="D20" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="37"/>
       <c r="J20" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L20" s="31"/>
       <c r="M20" s="31"/>
@@ -4166,7 +4157,7 @@
       <c r="R20" s="32"/>
       <c r="S20" s="33"/>
       <c r="T20" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,20 +4171,20 @@
         <v>51</v>
       </c>
       <c r="D21" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="F21" s="35"/>
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
       <c r="I21" s="37"/>
       <c r="J21" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L21" s="31"/>
       <c r="M21" s="31"/>
@@ -4204,7 +4195,7 @@
       <c r="R21" s="32"/>
       <c r="S21" s="33"/>
       <c r="T21" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4218,20 +4209,20 @@
         <v>51</v>
       </c>
       <c r="D22" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>97</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>98</v>
       </c>
       <c r="F22" s="35"/>
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="37"/>
       <c r="J22" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L22" s="31"/>
       <c r="M22" s="31"/>
@@ -4242,7 +4233,7 @@
       <c r="R22" s="32"/>
       <c r="S22" s="33"/>
       <c r="T22" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4256,20 +4247,20 @@
         <v>51</v>
       </c>
       <c r="D23" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="28" t="s">
         <v>99</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>100</v>
       </c>
       <c r="F23" s="35"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="37"/>
       <c r="J23" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L23" s="31"/>
       <c r="M23" s="31"/>
@@ -4280,7 +4271,7 @@
       <c r="R23" s="32"/>
       <c r="S23" s="33"/>
       <c r="T23" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4294,20 +4285,20 @@
         <v>51</v>
       </c>
       <c r="D24" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>103</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
       <c r="I24" s="37"/>
       <c r="J24" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L24" s="31"/>
       <c r="M24" s="31"/>
@@ -4318,7 +4309,7 @@
       <c r="R24" s="32"/>
       <c r="S24" s="33"/>
       <c r="T24" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4332,20 +4323,20 @@
         <v>51</v>
       </c>
       <c r="D25" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="28" t="s">
         <v>105</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>106</v>
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
       <c r="J25" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L25" s="31"/>
       <c r="M25" s="31"/>
@@ -4356,7 +4347,7 @@
       <c r="R25" s="32"/>
       <c r="S25" s="33"/>
       <c r="T25" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4370,20 +4361,20 @@
         <v>51</v>
       </c>
       <c r="D26" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="28" t="s">
         <v>107</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>108</v>
       </c>
       <c r="F26" s="35"/>
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
       <c r="J26" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K26" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L26" s="31"/>
       <c r="M26" s="31"/>
@@ -4394,7 +4385,7 @@
       <c r="R26" s="32"/>
       <c r="S26" s="33"/>
       <c r="T26" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4408,20 +4399,20 @@
         <v>51</v>
       </c>
       <c r="D27" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="28" t="s">
         <v>109</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>110</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
       <c r="J27" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K27" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L27" s="31"/>
       <c r="M27" s="31"/>
@@ -4432,7 +4423,7 @@
       <c r="R27" s="32"/>
       <c r="S27" s="33"/>
       <c r="T27" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,20 +4437,20 @@
         <v>51</v>
       </c>
       <c r="D28" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="28" t="s">
         <v>111</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>112</v>
       </c>
       <c r="F28" s="35"/>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="37"/>
       <c r="J28" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K28" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L28" s="31"/>
       <c r="M28" s="31"/>
@@ -4470,7 +4461,7 @@
       <c r="R28" s="32"/>
       <c r="S28" s="33"/>
       <c r="T28" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14465,10 +14456,10 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="102"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.86"/>
@@ -14484,10 +14475,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14495,125 +14486,125 @@
         <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="38" t="s">
         <v>116</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="38" t="s">
         <v>119</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="39" t="s">
         <v>122</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="38" t="s">
         <v>125</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="39" t="s">
         <v>128</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="39" t="s">
         <v>131</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="39" t="s">
         <v>134</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="39" t="s">
         <v>137</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="38" t="n">
         <v>191</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14621,111 +14612,111 @@
         <v>51</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" s="38" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="38" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="38" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="38" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="38" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" s="38" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="38" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="38" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14733,111 +14724,111 @@
         <v>51</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C19" s="38" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C20" s="38" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" s="38" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="38" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C23" s="38" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" s="38" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C25" s="38" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" s="38" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14845,111 +14836,111 @@
         <v>51</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="38" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="38" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C29" s="38" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C30" s="38" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C31" s="38" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C32" s="38" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C33" s="38" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C34" s="38" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14957,7 +14948,7 @@
         <v>51</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" s="38" t="n">
         <v>195</v>
@@ -14968,10 +14959,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" s="38" t="n">
         <v>211</v>
@@ -14982,10 +14973,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C37" s="38" t="n">
         <v>227</v>
@@ -14996,10 +14987,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" s="38" t="n">
         <v>243</v>
@@ -15010,10 +15001,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39" s="38" t="n">
         <v>259</v>
@@ -15024,10 +15015,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="38" t="n">
         <v>275</v>
@@ -15038,10 +15029,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C41" s="38" t="n">
         <v>291</v>
@@ -15052,10 +15043,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C42" s="38" t="n">
         <v>307</v>
@@ -15069,7 +15060,7 @@
         <v>51</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" s="38" t="n">
         <v>196</v>
@@ -15080,10 +15071,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C44" s="38" t="n">
         <v>212</v>
@@ -15094,10 +15085,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C45" s="38" t="n">
         <v>228</v>
@@ -15108,10 +15099,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C46" s="38" t="n">
         <v>244</v>
@@ -15122,10 +15113,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C47" s="38" t="n">
         <v>260</v>
@@ -15136,10 +15127,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" s="38" t="n">
         <v>276</v>
@@ -15150,10 +15141,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C49" s="38" t="n">
         <v>292</v>
@@ -15164,10 +15155,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C50" s="38" t="n">
         <v>308</v>
@@ -16145,7 +16136,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -16162,18 +16153,18 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Accreditamento Lettera di Dimissione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INNOGEASRLX/Innogea srl/CareMed/1.0/accreditamento-checklist_V8.1.2.xlsx
+++ b/GATEWAY/A1#111INNOGEASRLX/Innogea srl/CareMed/1.0/accreditamento-checklist_V8.1.2.xlsx
@@ -15,8 +15,9 @@
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$28</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$47</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="filtro" vbProcedure="false">TestCases!$A$9:$S$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">TestCases!$A$9:$T$28</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="218">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -593,6 +594,184 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
+    <t xml:space="preserve">LDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5dab29cbf040a9f7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.5.4.4b32b5f866bacae189fef7a96e213924d38c71202d8c8f121c47c7d8a307a1c3.2da0df9a6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5b1be6b07fcdb364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.5.4.f73a318b27b3c51ae65cd4e64c63987c98fafb2b3da99aadce0d8bf93e67acd4.9cb72349be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7c50bb15f7c66ffb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.190.4.5.4.f471faf3b361ba35abeee3a466d29264f060800cf8e1a724d97df1f6cd176191.d2a35091f8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’implementazione della generazione della sezione “Inquadramento clinico iniziale” richiede una rifattorizzazione di alcune parti del software che é rimandata a una versione successiva di CareMed. Non è quindi possibile generare un CDA2 che soddisfi il test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_LDO_TIMEOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT5_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT7_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non è possibile firmare digitalmente una relazione di dimissione in CareMed in mancanza di questa informazione. Nessuna trasmissione è quindi possibile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT11_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT13_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’implementazione della generazione della sezione “Inquadramento clinico iniziale” richiede una rifattorizzazione di alcune parti del software che é rimandata a una versione successiva di CareMed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT14_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non è possibile generare in CareMed 
+una terapia farmacologica alla dimissione 
+Priva dell’informazione richiesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT15_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non è prevista, al momento in CareMed, la codifica del motivo del ricovero, è possibile solo inserire testo libero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La terapia farmacologica alla dimissione, se presente, è compilata a partire dal prontuario farmaceutico interno a CareMed. Non essendo possibile inserire manualmente un farmaco nello stesso prontuario se non è disponibile il codice ATC (l’unico codice gestito al momento) non è possibile riprodurre il test case.</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
   </si>
   <si>
@@ -606,9 +785,6 @@
   </si>
   <si>
     <t xml:space="preserve">28,36,44,52,53,54,55,56,57,58,59,60,61,62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDO</t>
   </si>
   <si>
     <t xml:space="preserve">6,7,8,9</t>
@@ -3447,17 +3623,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="K14" activeCellId="0" sqref="K14"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3932,7 +4108,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="n">
         <v>28</v>
       </c>
@@ -3970,7 +4146,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="n">
         <v>36</v>
       </c>
@@ -4008,7 +4184,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="26" t="n">
         <v>44</v>
       </c>
@@ -4046,7 +4222,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="n">
         <v>52</v>
       </c>
@@ -4084,7 +4260,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="26" t="n">
         <v>53</v>
       </c>
@@ -4122,7 +4298,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="n">
         <v>54</v>
       </c>
@@ -4160,7 +4336,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="26" t="n">
         <v>55</v>
       </c>
@@ -4198,7 +4374,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="n">
         <v>56</v>
       </c>
@@ -4236,7 +4412,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="n">
         <v>57</v>
       </c>
@@ -4274,7 +4450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="n">
         <v>58</v>
       </c>
@@ -4312,7 +4488,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="n">
         <v>59</v>
       </c>
@@ -4350,7 +4526,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="n">
         <v>60</v>
       </c>
@@ -4388,7 +4564,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="n">
         <v>61</v>
       </c>
@@ -4426,7 +4602,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="n">
         <v>62</v>
       </c>
@@ -4464,328 +4640,744 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="14"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="14"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="14"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="14"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="14"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="14"/>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="14"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="14"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="14"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
-      <c r="Q38" s="12"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="14"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="13"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="14"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="12"/>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="13"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="14"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="14"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="14"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="13"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="14"/>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="13"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="14"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="13"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="14"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="12"/>
-      <c r="Q46" s="12"/>
-      <c r="R46" s="13"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="14"/>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="12"/>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="13"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="14"/>
+    <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="26" t="n">
+        <v>6</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="35" t="n">
+        <v>45104</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>20230627164006</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="26" t="n">
+        <v>7</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="35" t="n">
+        <v>45104</v>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>20230627164015</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="26" t="n">
+        <v>8</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="35" t="n">
+        <v>45104</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>20230627175016</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J31" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="26" t="n">
+        <v>9</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" s="35"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="33"/>
+      <c r="T32" s="34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="26" t="n">
+        <v>29</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="35"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="33"/>
+      <c r="T33" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="26" t="n">
+        <v>37</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="35"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="33"/>
+      <c r="T34" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="26" t="n">
+        <v>45</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="35"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="33"/>
+      <c r="T35" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="26" t="n">
+        <v>63</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="35"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="31"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="33"/>
+      <c r="T36" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="26" t="n">
+        <v>64</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="35"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="33"/>
+      <c r="T37" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="26" t="n">
+        <v>65</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="35"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="33"/>
+      <c r="T38" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="26" t="n">
+        <v>66</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="35"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="33"/>
+      <c r="T39" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="26" t="n">
+        <v>67</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="35"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="33"/>
+      <c r="T40" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="26" t="n">
+        <v>68</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="35"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="33"/>
+      <c r="T41" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="26" t="n">
+        <v>69</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" s="35"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+      <c r="N42" s="31"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="33"/>
+      <c r="T42" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="26" t="n">
+        <v>70</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" s="35"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="26" t="n">
+        <v>71</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="35"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="31"/>
+      <c r="Q44" s="31"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="33"/>
+      <c r="T44" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="26" t="n">
+        <v>72</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="35"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M45" s="31"/>
+      <c r="N45" s="31"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="33"/>
+      <c r="T45" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="26" t="n">
+        <v>73</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="F46" s="35"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="33"/>
+      <c r="T46" s="34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="26" t="n">
+        <v>74</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F47" s="35"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="33"/>
+      <c r="T47" s="34" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F48" s="11"/>
@@ -14407,9 +14999,14 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A9:T28">
-    <sortState ref="A10:T28">
-      <sortCondition ref="A10:A28" customList=""/>
+  <autoFilter ref="A9:T47">
+    <filterColumn colId="19">
+      <customFilters and="true">
+        <customFilter operator="equal" val="OK"/>
+      </customFilters>
+    </filterColumn>
+    <sortState ref="A10:T47">
+      <sortCondition ref="A10:A47" customList=""/>
     </sortState>
   </autoFilter>
   <mergeCells count="7">
@@ -14421,13 +15018,21 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10:J28 L10:M28 O10:O28" type="list">
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10:J29 L10:M28 O10:O28 J30:J47" type="list">
       <formula1>Sheet1!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q10:Q28" type="list">
       <formula1>Sheet1!$A$2:$A$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L29:M44 O29:O47 M45 L46:M47" type="list">
+      <formula1>#REF!</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q29:Q47" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -14475,10 +15080,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14486,125 +15091,125 @@
         <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>134</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>136</v>
+        <v>183</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C10" s="38" t="n">
         <v>191</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14612,111 +15217,111 @@
         <v>51</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C11" s="38" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C12" s="38" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C13" s="38" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C14" s="38" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C15" s="38" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>145</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C16" s="38" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>146</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C17" s="38" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>147</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C18" s="38" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>148</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14724,111 +15329,111 @@
         <v>51</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C19" s="38" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C20" s="38" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C21" s="38" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C22" s="38" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C23" s="38" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C24" s="38" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>155</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C25" s="38" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C26" s="38" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14836,111 +15441,111 @@
         <v>51</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C27" s="38" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C28" s="38" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C29" s="38" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C30" s="38" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C31" s="38" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C32" s="38" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>164</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C33" s="38" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
       <c r="C34" s="38" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14948,7 +15553,7 @@
         <v>51</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C35" s="38" t="n">
         <v>195</v>
@@ -14959,10 +15564,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C36" s="38" t="n">
         <v>211</v>
@@ -14973,10 +15578,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C37" s="38" t="n">
         <v>227</v>
@@ -14987,10 +15592,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C38" s="38" t="n">
         <v>243</v>
@@ -15001,10 +15606,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C39" s="38" t="n">
         <v>259</v>
@@ -15015,10 +15620,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C40" s="38" t="n">
         <v>275</v>
@@ -15029,10 +15634,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C41" s="38" t="n">
         <v>291</v>
@@ -15043,10 +15648,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C42" s="38" t="n">
         <v>307</v>
@@ -15060,7 +15665,7 @@
         <v>51</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C43" s="38" t="n">
         <v>196</v>
@@ -15071,10 +15676,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C44" s="38" t="n">
         <v>212</v>
@@ -15085,10 +15690,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C45" s="38" t="n">
         <v>228</v>
@@ -15099,10 +15704,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>123</v>
+        <v>170</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C46" s="38" t="n">
         <v>244</v>
@@ -15113,10 +15718,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C47" s="38" t="n">
         <v>260</v>
@@ -15127,10 +15732,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C48" s="38" t="n">
         <v>276</v>
@@ -15141,10 +15746,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C49" s="38" t="n">
         <v>292</v>
@@ -15155,10 +15760,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>168</v>
+        <v>215</v>
       </c>
       <c r="C50" s="38" t="n">
         <v>308</v>
@@ -16153,7 +16758,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>82</v>
@@ -16161,7 +16766,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Corretta razione di applicabilità test case con ID 83, 159 come richiesto via email il 21.7.2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111INNOGEASRLX/Innogea srl/CareMed/1.0/accreditamento-checklist_V8.1.2.xlsx
+++ b/GATEWAY/A1#111INNOGEASRLX/Innogea srl/CareMed/1.0/accreditamento-checklist_V8.1.2.xlsx
@@ -891,7 +891,7 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">L’inserimento della priorità della ricetta è obbligatorio in fase di accettazione della stessa. Non è possibile refertare se quest’informazione</t>
+    <t xml:space="preserve">infullfilmentof/order/id contiene sempre almeno l’identificativo dell’ordine interno, attribuito in fase di creazione della visita; se viene associata una prescrizione gli id saranno due. In nessun caso è possibile generare un referto XML che ne sia privo all’interno di CareMed.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT14_KO</t>
@@ -1926,7 +1926,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="230.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -3000,7 +3000,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -4104,14 +4104,14 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+      <selection pane="bottomRight" activeCell="A86" activeCellId="0" sqref="A86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
@@ -6448,7 +6448,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="26" t="n">
         <v>83</v>
       </c>
@@ -16519,7 +16519,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -18199,7 +18199,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>

</xml_diff>